<commit_message>
Cleaned up code, updated readme
</commit_message>
<xml_diff>
--- a/Overview.xlsx
+++ b/Overview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19350" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19350" windowHeight="8340" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="413">
   <si>
     <t>a</t>
   </si>
@@ -1257,13 +1257,19 @@
   </si>
   <si>
     <t>Lower ``4</t>
+  </si>
+  <si>
+    <t>] [ ] [</t>
+  </si>
+  <si>
+    <t>𝐀</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -1324,6 +1330,12 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color rgb="FF404040"/>
       <name val="Cambria"/>
@@ -1350,7 +1362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1397,6 +1409,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1407,8 +1420,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1692,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34:E35"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2240,7 +2253,9 @@
       <c r="C26" t="s">
         <v>165</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>411</v>
+      </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -2686,8 +2701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2707,10 +2722,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>407</v>
       </c>
       <c r="C1" s="29"/>
@@ -3974,10 +3989,10 @@
       <c r="E2" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="38" t="s">
         <v>377</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="33" t="s">
         <v>335</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -4052,7 +4067,7 @@
       <c r="B5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="33" t="s">
         <v>181</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -4075,7 +4090,7 @@
       <c r="B6" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="33" t="s">
         <v>183</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -4098,7 +4113,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="34" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -4130,7 +4145,7 @@
       <c r="A8" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="38" t="s">
         <v>334</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -4161,19 +4176,19 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="34"/>
-      <c r="E11" s="35" t="s">
+      <c r="D11" s="35"/>
+      <c r="E11" s="36" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F12" s="36"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="33"/>
+      <c r="E17" s="34"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="33"/>
+      <c r="B19" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4185,7 +4200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4267,7 +4282,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4276,6 +4291,9 @@
       </c>
       <c r="C7" t="s">
         <v>383</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4377,7 +4395,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -4388,7 +4406,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -4398,8 +4416,11 @@
       <c r="C18" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -4413,7 +4434,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -4424,7 +4445,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -4435,7 +4456,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>297</v>
       </c>
@@ -4446,7 +4467,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -4457,7 +4478,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>304</v>
       </c>
@@ -4468,7 +4489,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -4481,5 +4502,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>